<commit_message>
Actualizacion de documentos ficha y matriz
Se agrega la actualizacion de la Ficha de proyecto y La de Matriz
</commit_message>
<xml_diff>
--- a/Documentacion/Formato Matriz de requisitos.xlsx
+++ b/Documentacion/Formato Matriz de requisitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emacr\Desktop\Proyecto\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915A5B83-2001-4282-84CC-EDADEFD8F55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561BE620-487F-44CF-A10A-C5B8F46B0ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4440" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" RF" sheetId="1" r:id="rId1"/>
@@ -1611,7 +1611,6 @@
     <xf numFmtId="0" fontId="19" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1686,39 +1685,27 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1757,25 +1744,48 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1785,19 +1795,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1832,12 +1831,13 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2100,7 +2100,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2108,7 +2108,7 @@
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="57.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" customWidth="1"/>
+    <col min="4" max="4" width="90.5703125" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" customWidth="1"/>
     <col min="6" max="6" width="60.5703125" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" customWidth="1"/>
@@ -2190,19 +2190,19 @@
     <row r="5" spans="1:27" ht="30" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
-      <c r="C5" s="110" t="s">
+      <c r="C5" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="111"/>
-      <c r="E5" s="110" t="s">
+      <c r="D5" s="87"/>
+      <c r="E5" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="111"/>
-      <c r="G5" s="110" t="s">
+      <c r="F5" s="87"/>
+      <c r="G5" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="112"/>
-      <c r="I5" s="59" t="s">
+      <c r="H5" s="88"/>
+      <c r="I5" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J5" s="12"/>
@@ -2246,10 +2246,10 @@
       <c r="G6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="82" t="s">
+      <c r="H6" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="59" t="s">
+      <c r="I6" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J6" s="15"/>
@@ -2272,10 +2272,10 @@
       <c r="AA6" s="15"/>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A7" s="85" t="s">
+      <c r="A7" s="105" t="s">
         <v>182</v>
       </c>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="89" t="s">
         <v>84</v>
       </c>
       <c r="C7" s="48" t="s">
@@ -2284,19 +2284,19 @@
       <c r="D7" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="F7" s="56" t="s">
+      <c r="F7" s="55" t="s">
         <v>152</v>
       </c>
-      <c r="G7" s="59">
+      <c r="G7" s="58">
         <v>1</v>
       </c>
-      <c r="H7" s="83" t="s">
+      <c r="H7" s="82" t="s">
         <v>188</v>
       </c>
-      <c r="I7" s="59" t="s">
+      <c r="I7" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J7" s="15"/>
@@ -2319,27 +2319,27 @@
       <c r="AA7" s="15"/>
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A8" s="86"/>
-      <c r="B8" s="96"/>
+      <c r="A8" s="106"/>
+      <c r="B8" s="89"/>
       <c r="C8" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="145" t="s">
+      <c r="D8" s="84" t="s">
         <v>88</v>
       </c>
       <c r="E8" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="56" t="s">
+      <c r="F8" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="G8" s="59">
+      <c r="G8" s="58">
         <v>2</v>
       </c>
-      <c r="H8" s="61" t="s">
+      <c r="H8" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J8" s="15"/>
@@ -2362,27 +2362,27 @@
       <c r="AA8" s="15"/>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A9" s="86"/>
-      <c r="B9" s="96"/>
+      <c r="A9" s="106"/>
+      <c r="B9" s="89"/>
       <c r="C9" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="145" t="s">
+      <c r="D9" s="84" t="s">
         <v>90</v>
       </c>
       <c r="E9" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="55" t="s">
         <v>154</v>
       </c>
-      <c r="G9" s="59">
+      <c r="G9" s="58">
         <v>3</v>
       </c>
-      <c r="H9" s="61" t="s">
+      <c r="H9" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J9" s="15"/>
@@ -2405,31 +2405,31 @@
       <c r="AA9" s="15"/>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="90" t="s">
         <v>183</v>
       </c>
-      <c r="B10" s="87" t="s">
+      <c r="B10" s="90" t="s">
         <v>77</v>
       </c>
       <c r="C10" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="146" t="s">
+      <c r="D10" s="85" t="s">
         <v>79</v>
       </c>
       <c r="E10" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="55" t="s">
         <v>155</v>
       </c>
-      <c r="G10" s="59">
+      <c r="G10" s="58">
         <v>4</v>
       </c>
-      <c r="H10" s="61" t="s">
+      <c r="H10" s="60" t="s">
         <v>191</v>
       </c>
-      <c r="I10" s="59" t="s">
+      <c r="I10" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J10" s="15"/>
@@ -2452,8 +2452,8 @@
       <c r="AA10" s="15"/>
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A11" s="87"/>
-      <c r="B11" s="97"/>
+      <c r="A11" s="90"/>
+      <c r="B11" s="91"/>
       <c r="C11" s="51" t="s">
         <v>87</v>
       </c>
@@ -2463,16 +2463,16 @@
       <c r="E11" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="F11" s="56" t="s">
+      <c r="F11" s="55" t="s">
         <v>156</v>
       </c>
-      <c r="G11" s="59">
+      <c r="G11" s="58">
         <v>5</v>
       </c>
-      <c r="H11" s="62" t="s">
+      <c r="H11" s="61" t="s">
         <v>192</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J11" s="15"/>
@@ -2495,27 +2495,27 @@
       <c r="AA11" s="15"/>
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A12" s="87"/>
-      <c r="B12" s="89"/>
+      <c r="A12" s="90"/>
+      <c r="B12" s="92"/>
       <c r="C12" s="51" t="s">
         <v>89</v>
       </c>
       <c r="D12" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="F12" s="56" t="s">
+      <c r="F12" s="55" t="s">
         <v>157</v>
       </c>
-      <c r="G12" s="59">
+      <c r="G12" s="58">
         <v>6</v>
       </c>
-      <c r="H12" s="62" t="s">
+      <c r="H12" s="61" t="s">
         <v>193</v>
       </c>
-      <c r="I12" s="59" t="s">
+      <c r="I12" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J12" s="15"/>
@@ -2538,31 +2538,31 @@
       <c r="AA12" s="15"/>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="107" t="s">
         <v>184</v>
       </c>
-      <c r="B13" s="100" t="s">
+      <c r="B13" s="95" t="s">
         <v>113</v>
       </c>
       <c r="C13" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="145" t="s">
+      <c r="D13" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="E13" s="58" t="s">
+      <c r="E13" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="55" t="s">
         <v>158</v>
       </c>
-      <c r="G13" s="59">
+      <c r="G13" s="58">
         <v>7</v>
       </c>
-      <c r="H13" s="62" t="s">
+      <c r="H13" s="61" t="s">
         <v>194</v>
       </c>
-      <c r="I13" s="59" t="s">
+      <c r="I13" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J13" s="15"/>
@@ -2585,27 +2585,27 @@
       <c r="AA13" s="15"/>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A14" s="89"/>
-      <c r="B14" s="100"/>
+      <c r="A14" s="92"/>
+      <c r="B14" s="95"/>
       <c r="C14" s="51" t="s">
         <v>93</v>
       </c>
       <c r="D14" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="58" t="s">
+      <c r="E14" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="F14" s="56" t="s">
+      <c r="F14" s="55" t="s">
         <v>159</v>
       </c>
-      <c r="G14" s="59">
+      <c r="G14" s="58">
         <v>8</v>
       </c>
-      <c r="H14" s="62" t="s">
+      <c r="H14" s="61" t="s">
         <v>195</v>
       </c>
-      <c r="I14" s="59" t="s">
+      <c r="I14" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J14" s="15"/>
@@ -2628,10 +2628,10 @@
       <c r="AA14" s="15"/>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A15" s="87" t="s">
+      <c r="A15" s="90" t="s">
         <v>185</v>
       </c>
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="96" t="s">
         <v>129</v>
       </c>
       <c r="C15" s="50" t="s">
@@ -2640,19 +2640,19 @@
       <c r="D15" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="58" t="s">
+      <c r="E15" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="55" t="s">
         <v>160</v>
       </c>
-      <c r="G15" s="59">
+      <c r="G15" s="58">
         <v>9</v>
       </c>
-      <c r="H15" s="62" t="s">
+      <c r="H15" s="61" t="s">
         <v>196</v>
       </c>
-      <c r="I15" s="59" t="s">
+      <c r="I15" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J15" s="15"/>
@@ -2675,27 +2675,27 @@
       <c r="AA15" s="15"/>
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A16" s="87"/>
-      <c r="B16" s="102"/>
+      <c r="A16" s="90"/>
+      <c r="B16" s="97"/>
       <c r="C16" s="50" t="s">
         <v>95</v>
       </c>
       <c r="D16" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="58" t="s">
+      <c r="E16" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="F16" s="56" t="s">
+      <c r="F16" s="55" t="s">
         <v>161</v>
       </c>
-      <c r="G16" s="59">
+      <c r="G16" s="58">
         <v>10</v>
       </c>
-      <c r="H16" s="62" t="s">
+      <c r="H16" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="I16" s="59" t="s">
+      <c r="I16" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J16" s="15"/>
@@ -2718,27 +2718,27 @@
       <c r="AA16" s="15"/>
     </row>
     <row r="17" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A17" s="87"/>
-      <c r="B17" s="102"/>
+      <c r="A17" s="90"/>
+      <c r="B17" s="97"/>
       <c r="C17" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" s="146" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="F17" s="56" t="s">
+      <c r="F17" s="55" t="s">
         <v>162</v>
       </c>
-      <c r="G17" s="60">
+      <c r="G17" s="59">
         <v>11</v>
       </c>
-      <c r="H17" s="62" t="s">
+      <c r="H17" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="I17" s="59" t="s">
+      <c r="I17" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J17" s="15"/>
@@ -2761,27 +2761,27 @@
       <c r="AA17" s="15"/>
     </row>
     <row r="18" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A18" s="87"/>
-      <c r="B18" s="103"/>
+      <c r="A18" s="90"/>
+      <c r="B18" s="98"/>
       <c r="C18" s="51" t="s">
         <v>104</v>
       </c>
       <c r="D18" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="58" t="s">
+      <c r="E18" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="F18" s="56" t="s">
+      <c r="F18" s="55" t="s">
         <v>163</v>
       </c>
-      <c r="G18" s="60">
+      <c r="G18" s="59">
         <v>12</v>
       </c>
-      <c r="H18" s="62" t="s">
+      <c r="H18" s="61" t="s">
         <v>199</v>
       </c>
-      <c r="I18" s="59" t="s">
+      <c r="I18" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J18" s="15"/>
@@ -2804,10 +2804,10 @@
       <c r="AA18" s="15"/>
     </row>
     <row r="19" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A19" s="94" t="s">
+      <c r="A19" s="112" t="s">
         <v>186</v>
       </c>
-      <c r="B19" s="104" t="s">
+      <c r="B19" s="99" t="s">
         <v>99</v>
       </c>
       <c r="C19" s="51" t="s">
@@ -2816,19 +2816,19 @@
       <c r="D19" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="58" t="s">
+      <c r="E19" s="57" t="s">
         <v>142</v>
       </c>
-      <c r="F19" s="56" t="s">
+      <c r="F19" s="55" t="s">
         <v>164</v>
       </c>
-      <c r="G19" s="60">
+      <c r="G19" s="59">
         <v>13</v>
       </c>
-      <c r="H19" s="62" t="s">
+      <c r="H19" s="61" t="s">
         <v>200</v>
       </c>
-      <c r="I19" s="59" t="s">
+      <c r="I19" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J19" s="15"/>
@@ -2851,27 +2851,27 @@
       <c r="AA19" s="15"/>
     </row>
     <row r="20" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A20" s="94"/>
-      <c r="B20" s="105"/>
+      <c r="A20" s="112"/>
+      <c r="B20" s="100"/>
       <c r="C20" s="51" t="s">
         <v>110</v>
       </c>
       <c r="D20" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="58" t="s">
+      <c r="E20" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="F20" s="56" t="s">
+      <c r="F20" s="55" t="s">
         <v>165</v>
       </c>
-      <c r="G20" s="60">
+      <c r="G20" s="59">
         <v>14</v>
       </c>
-      <c r="H20" s="62" t="s">
+      <c r="H20" s="61" t="s">
         <v>201</v>
       </c>
-      <c r="I20" s="59" t="s">
+      <c r="I20" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J20" s="15"/>
@@ -2894,27 +2894,27 @@
       <c r="AA20" s="15"/>
     </row>
     <row r="21" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A21" s="94"/>
-      <c r="B21" s="106"/>
+      <c r="A21" s="112"/>
+      <c r="B21" s="101"/>
       <c r="C21" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="58" t="s">
+      <c r="E21" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="F21" s="56" t="s">
+      <c r="F21" s="55" t="s">
         <v>166</v>
       </c>
-      <c r="G21" s="60">
+      <c r="G21" s="59">
         <v>15</v>
       </c>
-      <c r="H21" s="62" t="s">
+      <c r="H21" s="61" t="s">
         <v>202</v>
       </c>
-      <c r="I21" s="59" t="s">
+      <c r="I21" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J21" s="15"/>
@@ -2937,31 +2937,31 @@
       <c r="AA21" s="15"/>
     </row>
     <row r="22" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="112" t="s">
         <v>187</v>
       </c>
-      <c r="B22" s="107" t="s">
+      <c r="B22" s="102" t="s">
         <v>106</v>
       </c>
       <c r="C22" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="54" t="s">
+      <c r="D22" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="58" t="s">
+      <c r="E22" s="57" t="s">
         <v>145</v>
       </c>
-      <c r="F22" s="56" t="s">
+      <c r="F22" s="55" t="s">
         <v>167</v>
       </c>
-      <c r="G22" s="60">
+      <c r="G22" s="59">
         <v>16</v>
       </c>
-      <c r="H22" s="62" t="s">
+      <c r="H22" s="61" t="s">
         <v>203</v>
       </c>
-      <c r="I22" s="59" t="s">
+      <c r="I22" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J22" s="15"/>
@@ -2984,27 +2984,27 @@
       <c r="AA22" s="15"/>
     </row>
     <row r="23" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A23" s="94"/>
-      <c r="B23" s="108"/>
+      <c r="A23" s="112"/>
+      <c r="B23" s="103"/>
       <c r="C23" s="51" t="s">
         <v>116</v>
       </c>
       <c r="D23" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="E23" s="58" t="s">
+      <c r="E23" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="F23" s="56" t="s">
+      <c r="F23" s="55" t="s">
         <v>168</v>
       </c>
-      <c r="G23" s="60">
+      <c r="G23" s="59">
         <v>17</v>
       </c>
-      <c r="H23" s="62" t="s">
+      <c r="H23" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="I23" s="59" t="s">
+      <c r="I23" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J23" s="15"/>
@@ -3027,27 +3027,27 @@
       <c r="AA23" s="15"/>
     </row>
     <row r="24" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A24" s="94"/>
-      <c r="B24" s="109"/>
+      <c r="A24" s="112"/>
+      <c r="B24" s="104"/>
       <c r="C24" s="51" t="s">
         <v>117</v>
       </c>
       <c r="D24" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="58" t="s">
+      <c r="E24" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="F24" s="56" t="s">
+      <c r="F24" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="G24" s="60">
+      <c r="G24" s="59">
         <v>18</v>
       </c>
-      <c r="H24" s="62" t="s">
+      <c r="H24" s="61" t="s">
         <v>205</v>
       </c>
-      <c r="I24" s="59" t="s">
+      <c r="I24" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J24" s="15"/>
@@ -3070,31 +3070,31 @@
       <c r="AA24" s="15"/>
     </row>
     <row r="25" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="B25" s="98" t="s">
+      <c r="B25" s="93" t="s">
         <v>118</v>
       </c>
       <c r="C25" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="146" t="s">
+      <c r="D25" s="85" t="s">
         <v>119</v>
       </c>
-      <c r="E25" s="58" t="s">
+      <c r="E25" s="57" t="s">
         <v>148</v>
       </c>
-      <c r="F25" s="56" t="s">
+      <c r="F25" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="G25" s="60">
+      <c r="G25" s="59">
         <v>19</v>
       </c>
-      <c r="H25" s="62" t="s">
+      <c r="H25" s="61" t="s">
         <v>206</v>
       </c>
-      <c r="I25" s="59" t="s">
+      <c r="I25" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J25" s="15"/>
@@ -3117,27 +3117,27 @@
       <c r="AA25" s="15"/>
     </row>
     <row r="26" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A26" s="94"/>
-      <c r="B26" s="99"/>
+      <c r="A26" s="112"/>
+      <c r="B26" s="94"/>
       <c r="C26" s="50" t="s">
         <v>124</v>
       </c>
       <c r="D26" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="E26" s="58" t="s">
+      <c r="E26" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="F26" s="56" t="s">
+      <c r="F26" s="55" t="s">
         <v>171</v>
       </c>
-      <c r="G26" s="60">
+      <c r="G26" s="59">
         <v>20</v>
       </c>
-      <c r="H26" s="84" t="s">
+      <c r="H26" s="83" t="s">
         <v>207</v>
       </c>
-      <c r="I26" s="59" t="s">
+      <c r="I26" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J26" s="15"/>
@@ -3160,27 +3160,27 @@
       <c r="AA26" s="15"/>
     </row>
     <row r="27" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A27" s="94"/>
-      <c r="B27" s="99"/>
+      <c r="A27" s="112"/>
+      <c r="B27" s="94"/>
       <c r="C27" s="50" t="s">
         <v>125</v>
       </c>
       <c r="D27" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="E27" s="58" t="s">
+      <c r="E27" s="57" t="s">
         <v>150</v>
       </c>
-      <c r="F27" s="56" t="s">
+      <c r="F27" s="55" t="s">
         <v>172</v>
       </c>
-      <c r="G27" s="60">
+      <c r="G27" s="59">
         <v>21</v>
       </c>
-      <c r="H27" s="84" t="s">
+      <c r="H27" s="83" t="s">
         <v>208</v>
       </c>
-      <c r="I27" s="59" t="s">
+      <c r="I27" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J27" s="15"/>
@@ -3203,27 +3203,27 @@
       <c r="AA27" s="15"/>
     </row>
     <row r="28" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A28" s="94"/>
-      <c r="B28" s="99"/>
-      <c r="C28" s="65" t="s">
+      <c r="A28" s="112"/>
+      <c r="B28" s="94"/>
+      <c r="C28" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="D28" s="66" t="s">
+      <c r="D28" s="65" t="s">
         <v>122</v>
       </c>
-      <c r="E28" s="67" t="s">
+      <c r="E28" s="66" t="s">
         <v>151</v>
       </c>
-      <c r="F28" s="68" t="s">
+      <c r="F28" s="67" t="s">
         <v>173</v>
       </c>
-      <c r="G28" s="69">
+      <c r="G28" s="68">
         <v>22</v>
       </c>
-      <c r="H28" s="84" t="s">
+      <c r="H28" s="83" t="s">
         <v>209</v>
       </c>
-      <c r="I28" s="59" t="s">
+      <c r="I28" s="58" t="s">
         <v>210</v>
       </c>
       <c r="J28" s="15"/>
@@ -3246,14 +3246,14 @@
       <c r="AA28" s="15"/>
     </row>
     <row r="29" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A29" s="95"/>
-      <c r="B29" s="64"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="71"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="64"/>
+      <c r="A29" s="113"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="63"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
@@ -3275,14 +3275,14 @@
       <c r="AA29" s="15"/>
     </row>
     <row r="30" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A30" s="95"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="73"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="63"/>
+      <c r="A30" s="113"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="62"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
@@ -3304,14 +3304,14 @@
       <c r="AA30" s="15"/>
     </row>
     <row r="31" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A31" s="95"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="70"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="64"/>
+      <c r="A31" s="113"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="63"/>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
@@ -3333,14 +3333,14 @@
       <c r="AA31" s="15"/>
     </row>
     <row r="32" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A32" s="95"/>
-      <c r="B32" s="64"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="71"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="64"/>
+      <c r="A32" s="113"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="72"/>
+      <c r="H32" s="63"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
@@ -3362,14 +3362,14 @@
       <c r="AA32" s="15"/>
     </row>
     <row r="33" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A33" s="95"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="73"/>
-      <c r="G33" s="73"/>
-      <c r="H33" s="64"/>
+      <c r="A33" s="113"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="72"/>
+      <c r="G33" s="72"/>
+      <c r="H33" s="63"/>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
@@ -3391,14 +3391,14 @@
       <c r="AA33" s="15"/>
     </row>
     <row r="34" spans="1:27" ht="15" customHeight="1">
-      <c r="A34" s="93"/>
-      <c r="B34" s="74"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="76"/>
-      <c r="H34" s="63"/>
+      <c r="A34" s="111"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="62"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -3420,14 +3420,14 @@
       <c r="AA34" s="4"/>
     </row>
     <row r="35" spans="1:27" ht="15" customHeight="1">
-      <c r="A35" s="91"/>
-      <c r="B35" s="64"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="64"/>
+      <c r="A35" s="109"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="74"/>
+      <c r="E35" s="75"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="63"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -3449,14 +3449,14 @@
       <c r="AA35" s="4"/>
     </row>
     <row r="36" spans="1:27" ht="15" customHeight="1">
-      <c r="A36" s="91"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="70"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="64"/>
+      <c r="A36" s="109"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="75"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="63"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -3478,14 +3478,14 @@
       <c r="AA36" s="4"/>
     </row>
     <row r="37" spans="1:27" ht="15" customHeight="1">
-      <c r="A37" s="91"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="76"/>
-      <c r="H37" s="64"/>
+      <c r="A37" s="109"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="63"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -3507,14 +3507,14 @@
       <c r="AA37" s="4"/>
     </row>
     <row r="38" spans="1:27" ht="15" customHeight="1">
-      <c r="A38" s="91"/>
-      <c r="B38" s="64"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="75"/>
-      <c r="E38" s="76"/>
-      <c r="F38" s="76"/>
-      <c r="G38" s="76"/>
-      <c r="H38" s="64"/>
+      <c r="A38" s="109"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="75"/>
+      <c r="H38" s="63"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -3536,14 +3536,14 @@
       <c r="AA38" s="4"/>
     </row>
     <row r="39" spans="1:27" ht="15" customHeight="1">
-      <c r="A39" s="92"/>
-      <c r="B39" s="64"/>
-      <c r="C39" s="70"/>
-      <c r="D39" s="75"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="64"/>
+      <c r="A39" s="110"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="75"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="75"/>
+      <c r="H39" s="63"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -3565,14 +3565,14 @@
       <c r="AA39" s="4"/>
     </row>
     <row r="40" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A40" s="90"/>
-      <c r="B40" s="74"/>
-      <c r="C40" s="70"/>
-      <c r="D40" s="75"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="75"/>
-      <c r="G40" s="75"/>
-      <c r="H40" s="63"/>
+      <c r="A40" s="108"/>
+      <c r="B40" s="73"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="74"/>
+      <c r="G40" s="74"/>
+      <c r="H40" s="62"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -3594,14 +3594,14 @@
       <c r="AA40" s="4"/>
     </row>
     <row r="41" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A41" s="91"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="64"/>
+      <c r="A41" s="109"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="75"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="63"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -3623,14 +3623,14 @@
       <c r="AA41" s="4"/>
     </row>
     <row r="42" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A42" s="91"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="77"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="79"/>
-      <c r="G42" s="75"/>
-      <c r="H42" s="64"/>
+      <c r="A42" s="109"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="77"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="63"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -3652,14 +3652,14 @@
       <c r="AA42" s="4"/>
     </row>
     <row r="43" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A43" s="91"/>
-      <c r="B43" s="64"/>
-      <c r="C43" s="70"/>
-      <c r="D43" s="75"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="75"/>
-      <c r="G43" s="75"/>
-      <c r="H43" s="64"/>
+      <c r="A43" s="109"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="75"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="63"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -3681,14 +3681,14 @@
       <c r="AA43" s="4"/>
     </row>
     <row r="44" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A44" s="91"/>
-      <c r="B44" s="74"/>
-      <c r="C44" s="70"/>
-      <c r="D44" s="75"/>
-      <c r="E44" s="76"/>
-      <c r="F44" s="75"/>
-      <c r="G44" s="75"/>
-      <c r="H44" s="80"/>
+      <c r="A44" s="109"/>
+      <c r="B44" s="73"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="75"/>
+      <c r="F44" s="74"/>
+      <c r="G44" s="74"/>
+      <c r="H44" s="79"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -3710,14 +3710,14 @@
       <c r="AA44" s="4"/>
     </row>
     <row r="45" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A45" s="91"/>
-      <c r="B45" s="64"/>
-      <c r="C45" s="70"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="76"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="75"/>
-      <c r="H45" s="80"/>
+      <c r="A45" s="109"/>
+      <c r="B45" s="63"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="75"/>
+      <c r="F45" s="74"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="79"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -3739,14 +3739,14 @@
       <c r="AA45" s="4"/>
     </row>
     <row r="46" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A46" s="91"/>
-      <c r="B46" s="64"/>
-      <c r="C46" s="70"/>
-      <c r="D46" s="75"/>
-      <c r="E46" s="75"/>
-      <c r="F46" s="75"/>
-      <c r="G46" s="75"/>
-      <c r="H46" s="80"/>
+      <c r="A46" s="109"/>
+      <c r="B46" s="63"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="74"/>
+      <c r="G46" s="74"/>
+      <c r="H46" s="79"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -3768,14 +3768,14 @@
       <c r="AA46" s="4"/>
     </row>
     <row r="47" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A47" s="90"/>
-      <c r="B47" s="74"/>
-      <c r="C47" s="70"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="76"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="81"/>
+      <c r="A47" s="108"/>
+      <c r="B47" s="73"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="75"/>
+      <c r="F47" s="74"/>
+      <c r="G47" s="74"/>
+      <c r="H47" s="80"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
@@ -3797,14 +3797,14 @@
       <c r="AA47" s="4"/>
     </row>
     <row r="48" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A48" s="91"/>
-      <c r="B48" s="64"/>
-      <c r="C48" s="70"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="76"/>
-      <c r="F48" s="75"/>
-      <c r="G48" s="75"/>
-      <c r="H48" s="64"/>
+      <c r="A48" s="109"/>
+      <c r="B48" s="63"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="75"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="63"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -3826,14 +3826,14 @@
       <c r="AA48" s="4"/>
     </row>
     <row r="49" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A49" s="91"/>
-      <c r="B49" s="64"/>
-      <c r="C49" s="70"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="76"/>
-      <c r="F49" s="75"/>
-      <c r="G49" s="75"/>
-      <c r="H49" s="64"/>
+      <c r="A49" s="109"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="75"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="74"/>
+      <c r="H49" s="63"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
@@ -3855,14 +3855,14 @@
       <c r="AA49" s="4"/>
     </row>
     <row r="50" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A50" s="91"/>
-      <c r="B50" s="64"/>
-      <c r="C50" s="70"/>
-      <c r="D50" s="75"/>
-      <c r="E50" s="76"/>
-      <c r="F50" s="75"/>
-      <c r="G50" s="75"/>
-      <c r="H50" s="64"/>
+      <c r="A50" s="109"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="69"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="75"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="63"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -3884,14 +3884,14 @@
       <c r="AA50" s="4"/>
     </row>
     <row r="51" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A51" s="91"/>
-      <c r="B51" s="64"/>
-      <c r="C51" s="70"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="76"/>
-      <c r="F51" s="75"/>
-      <c r="G51" s="75"/>
-      <c r="H51" s="64"/>
+      <c r="A51" s="109"/>
+      <c r="B51" s="63"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="75"/>
+      <c r="F51" s="74"/>
+      <c r="G51" s="74"/>
+      <c r="H51" s="63"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -3913,14 +3913,14 @@
       <c r="AA51" s="4"/>
     </row>
     <row r="52" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A52" s="91"/>
-      <c r="B52" s="64"/>
-      <c r="C52" s="70"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="76"/>
-      <c r="F52" s="75"/>
-      <c r="G52" s="75"/>
-      <c r="H52" s="64"/>
+      <c r="A52" s="109"/>
+      <c r="B52" s="63"/>
+      <c r="C52" s="69"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="75"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="74"/>
+      <c r="H52" s="63"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
@@ -3942,14 +3942,14 @@
       <c r="AA52" s="4"/>
     </row>
     <row r="53" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A53" s="91"/>
-      <c r="B53" s="64"/>
-      <c r="C53" s="70"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="76"/>
-      <c r="F53" s="75"/>
-      <c r="G53" s="75"/>
-      <c r="H53" s="64"/>
+      <c r="A53" s="109"/>
+      <c r="B53" s="63"/>
+      <c r="C53" s="69"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="75"/>
+      <c r="F53" s="74"/>
+      <c r="G53" s="74"/>
+      <c r="H53" s="63"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -3971,14 +3971,14 @@
       <c r="AA53" s="4"/>
     </row>
     <row r="54" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A54" s="91"/>
-      <c r="B54" s="64"/>
-      <c r="C54" s="70"/>
-      <c r="D54" s="75"/>
-      <c r="E54" s="76"/>
-      <c r="F54" s="75"/>
-      <c r="G54" s="75"/>
-      <c r="H54" s="64"/>
+      <c r="A54" s="109"/>
+      <c r="B54" s="63"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="74"/>
+      <c r="E54" s="75"/>
+      <c r="F54" s="74"/>
+      <c r="G54" s="74"/>
+      <c r="H54" s="63"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -4000,14 +4000,14 @@
       <c r="AA54" s="4"/>
     </row>
     <row r="55" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A55" s="91"/>
-      <c r="B55" s="64"/>
-      <c r="C55" s="70"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="76"/>
-      <c r="F55" s="75"/>
-      <c r="G55" s="75"/>
-      <c r="H55" s="64"/>
+      <c r="A55" s="109"/>
+      <c r="B55" s="63"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="74"/>
+      <c r="E55" s="75"/>
+      <c r="F55" s="74"/>
+      <c r="G55" s="74"/>
+      <c r="H55" s="63"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -4029,14 +4029,14 @@
       <c r="AA55" s="4"/>
     </row>
     <row r="56" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A56" s="91"/>
-      <c r="B56" s="74"/>
-      <c r="C56" s="70"/>
-      <c r="D56" s="75"/>
-      <c r="E56" s="76"/>
-      <c r="F56" s="75"/>
-      <c r="G56" s="75"/>
-      <c r="H56" s="64"/>
+      <c r="A56" s="109"/>
+      <c r="B56" s="73"/>
+      <c r="C56" s="69"/>
+      <c r="D56" s="74"/>
+      <c r="E56" s="75"/>
+      <c r="F56" s="74"/>
+      <c r="G56" s="74"/>
+      <c r="H56" s="63"/>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
@@ -4058,14 +4058,14 @@
       <c r="AA56" s="4"/>
     </row>
     <row r="57" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A57" s="91"/>
-      <c r="B57" s="64"/>
-      <c r="C57" s="70"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="76"/>
-      <c r="F57" s="75"/>
-      <c r="G57" s="75"/>
-      <c r="H57" s="64"/>
+      <c r="A57" s="109"/>
+      <c r="B57" s="63"/>
+      <c r="C57" s="69"/>
+      <c r="D57" s="74"/>
+      <c r="E57" s="75"/>
+      <c r="F57" s="74"/>
+      <c r="G57" s="74"/>
+      <c r="H57" s="63"/>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -4087,14 +4087,14 @@
       <c r="AA57" s="4"/>
     </row>
     <row r="58" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A58" s="91"/>
-      <c r="B58" s="64"/>
-      <c r="C58" s="70"/>
-      <c r="D58" s="75"/>
-      <c r="E58" s="76"/>
-      <c r="F58" s="75"/>
-      <c r="G58" s="75"/>
-      <c r="H58" s="64"/>
+      <c r="A58" s="109"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="69"/>
+      <c r="D58" s="74"/>
+      <c r="E58" s="75"/>
+      <c r="F58" s="74"/>
+      <c r="G58" s="74"/>
+      <c r="H58" s="63"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -4116,14 +4116,14 @@
       <c r="AA58" s="4"/>
     </row>
     <row r="59" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A59" s="92"/>
-      <c r="B59" s="64"/>
-      <c r="C59" s="70"/>
-      <c r="D59" s="75"/>
-      <c r="E59" s="76"/>
-      <c r="F59" s="75"/>
-      <c r="G59" s="75"/>
-      <c r="H59" s="64"/>
+      <c r="A59" s="110"/>
+      <c r="B59" s="63"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="74"/>
+      <c r="E59" s="75"/>
+      <c r="F59" s="74"/>
+      <c r="G59" s="74"/>
+      <c r="H59" s="63"/>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -12710,16 +12710,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B22:B24"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A13:A14"/>
@@ -12731,6 +12721,16 @@
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12758,15 +12758,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="124"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="116"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -12788,14 +12788,14 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="111"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="16"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -12821,12 +12821,12 @@
       <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="125" t="s">
+      <c r="B3" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="111"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="87"/>
       <c r="F3" s="18" t="s">
         <v>9</v>
       </c>
@@ -12857,16 +12857,16 @@
       <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="113" t="s">
+      <c r="B4" s="118" t="s">
         <v>174</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="114" t="s">
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="117" t="s">
+      <c r="G4" s="122" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="4"/>
@@ -12893,12 +12893,12 @@
       <c r="A5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="113"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="91"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="109"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -12923,12 +12923,12 @@
       <c r="A6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="113"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="91"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="120"/>
+      <c r="G6" s="109"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -12953,12 +12953,12 @@
       <c r="A7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="113"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="115"/>
-      <c r="G7" s="91"/>
+      <c r="B7" s="118"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="109"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -12983,16 +12983,16 @@
       <c r="A8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="119" t="s">
+      <c r="B8" s="123" t="s">
         <v>175</v>
       </c>
-      <c r="C8" s="120"/>
-      <c r="D8" s="120"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="116" t="s">
+      <c r="C8" s="124"/>
+      <c r="D8" s="124"/>
+      <c r="E8" s="125"/>
+      <c r="F8" s="126" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="117" t="s">
+      <c r="G8" s="122" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="4"/>
@@ -13019,12 +13019,12 @@
       <c r="A9" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="113"/>
-      <c r="C9" s="112"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="111"/>
-      <c r="F9" s="115"/>
-      <c r="G9" s="91"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="121"/>
+      <c r="G9" s="109"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -13049,16 +13049,16 @@
       <c r="A10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="113" t="s">
+      <c r="B10" s="118" t="s">
         <v>176</v>
       </c>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="111"/>
-      <c r="F10" s="114" t="s">
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="119" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="117" t="s">
+      <c r="G10" s="122" t="s">
         <v>23</v>
       </c>
       <c r="H10" s="4"/>
@@ -13085,12 +13085,12 @@
       <c r="A11" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="113"/>
-      <c r="C11" s="112"/>
-      <c r="D11" s="112"/>
-      <c r="E11" s="111"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="91"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="87"/>
+      <c r="F11" s="120"/>
+      <c r="G11" s="109"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -13115,12 +13115,12 @@
       <c r="A12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="113"/>
-      <c r="C12" s="112"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="91"/>
+      <c r="B12" s="118"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="120"/>
+      <c r="G12" s="109"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -13145,12 +13145,12 @@
       <c r="A13" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="113"/>
-      <c r="C13" s="112"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="91"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="109"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -13175,16 +13175,16 @@
       <c r="A14" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="113" t="s">
+      <c r="B14" s="118" t="s">
         <v>177</v>
       </c>
-      <c r="C14" s="112"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="111"/>
-      <c r="F14" s="116" t="s">
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="117" t="s">
+      <c r="G14" s="122" t="s">
         <v>29</v>
       </c>
       <c r="I14" s="4"/>
@@ -13210,12 +13210,12 @@
       <c r="A15" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="113"/>
-      <c r="C15" s="112"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="111"/>
-      <c r="F15" s="115"/>
-      <c r="G15" s="91"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="109"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -13240,16 +13240,16 @@
       <c r="A16" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="113" t="s">
+      <c r="B16" s="118" t="s">
         <v>181</v>
       </c>
-      <c r="C16" s="112"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="111"/>
-      <c r="F16" s="114" t="s">
+      <c r="C16" s="88"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="117" t="s">
+      <c r="G16" s="122" t="s">
         <v>33</v>
       </c>
       <c r="H16" s="4"/>
@@ -13276,12 +13276,12 @@
       <c r="A17" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="113"/>
-      <c r="C17" s="112"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="111"/>
-      <c r="F17" s="115"/>
-      <c r="G17" s="91"/>
+      <c r="B17" s="118"/>
+      <c r="C17" s="88"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="121"/>
+      <c r="G17" s="109"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -13306,16 +13306,16 @@
       <c r="A18" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="113" t="s">
+      <c r="B18" s="118" t="s">
         <v>179</v>
       </c>
-      <c r="C18" s="112"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="116" t="s">
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="117" t="s">
+      <c r="G18" s="122" t="s">
         <v>37</v>
       </c>
       <c r="H18" s="4"/>
@@ -13342,12 +13342,12 @@
       <c r="A19" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="113"/>
-      <c r="C19" s="112"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="118"/>
-      <c r="G19" s="91"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="120"/>
+      <c r="G19" s="109"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -13372,12 +13372,12 @@
       <c r="A20" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="113"/>
-      <c r="C20" s="112"/>
-      <c r="D20" s="112"/>
-      <c r="E20" s="111"/>
-      <c r="F20" s="115"/>
-      <c r="G20" s="91"/>
+      <c r="B20" s="118"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="121"/>
+      <c r="G20" s="109"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -13402,16 +13402,16 @@
       <c r="A21" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="113" t="s">
+      <c r="B21" s="118" t="s">
         <v>180</v>
       </c>
-      <c r="C21" s="112"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="111"/>
-      <c r="F21" s="114" t="s">
+      <c r="C21" s="88"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="117" t="s">
+      <c r="G21" s="122" t="s">
         <v>42</v>
       </c>
       <c r="I21" s="4"/>
@@ -13437,12 +13437,12 @@
       <c r="A22" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="113"/>
-      <c r="C22" s="112"/>
-      <c r="D22" s="112"/>
-      <c r="E22" s="111"/>
-      <c r="F22" s="115"/>
-      <c r="G22" s="91"/>
+      <c r="B22" s="118"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="121"/>
+      <c r="G22" s="109"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -13467,16 +13467,16 @@
       <c r="A23" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="113" t="s">
+      <c r="B23" s="118" t="s">
         <v>178</v>
       </c>
-      <c r="C23" s="112"/>
-      <c r="D23" s="112"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="116" t="s">
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="117" t="s">
+      <c r="G23" s="122" t="s">
         <v>46</v>
       </c>
       <c r="H23" s="4"/>
@@ -13503,12 +13503,12 @@
       <c r="A24" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="113"/>
-      <c r="C24" s="112"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="111"/>
-      <c r="F24" s="115"/>
-      <c r="G24" s="91"/>
+      <c r="B24" s="118"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="121"/>
+      <c r="G24" s="109"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -22235,30 +22235,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="F21:F22"/>
@@ -22275,6 +22251,30 @@
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="G18:G20"/>
     <mergeCell ref="F18:F20"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -22315,36 +22315,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:111" ht="21.75" customHeight="1">
-      <c r="A1" s="128"/>
-      <c r="B1" s="129"/>
-      <c r="C1" s="133" t="s">
+      <c r="A1" s="127"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="132" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="134" t="s">
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="135"/>
-      <c r="L1" s="135"/>
-      <c r="M1" s="135"/>
-      <c r="N1" s="135"/>
-      <c r="O1" s="135"/>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="135"/>
-      <c r="R1" s="135"/>
-      <c r="S1" s="135"/>
-      <c r="T1" s="136"/>
-      <c r="U1" s="137" t="s">
+      <c r="K1" s="134"/>
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="134"/>
+      <c r="P1" s="134"/>
+      <c r="Q1" s="134"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
+      <c r="T1" s="135"/>
+      <c r="U1" s="136" t="s">
         <v>50</v>
       </c>
-      <c r="V1" s="138"/>
-      <c r="W1" s="138"/>
-      <c r="X1" s="139"/>
+      <c r="V1" s="137"/>
+      <c r="W1" s="137"/>
+      <c r="X1" s="138"/>
       <c r="Y1" s="23"/>
       <c r="Z1" s="23"/>
       <c r="AA1" s="23"/>
@@ -22434,8 +22434,8 @@
       <c r="DG1" s="24"/>
     </row>
     <row r="2" spans="1:111" ht="18.75" customHeight="1">
-      <c r="A2" s="129"/>
-      <c r="B2" s="129"/>
+      <c r="A2" s="128"/>
+      <c r="B2" s="128"/>
       <c r="C2" s="25" t="s">
         <v>51</v>
       </c>
@@ -22457,25 +22457,25 @@
       <c r="I2" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="140" t="s">
+      <c r="J2" s="139" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="135"/>
-      <c r="L2" s="136"/>
-      <c r="M2" s="140" t="s">
+      <c r="K2" s="134"/>
+      <c r="L2" s="135"/>
+      <c r="M2" s="139" t="s">
         <v>59</v>
       </c>
-      <c r="N2" s="136"/>
-      <c r="O2" s="140" t="s">
+      <c r="N2" s="135"/>
+      <c r="O2" s="139" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="135"/>
-      <c r="Q2" s="136"/>
-      <c r="R2" s="140" t="s">
+      <c r="P2" s="134"/>
+      <c r="Q2" s="135"/>
+      <c r="R2" s="139" t="s">
         <v>61</v>
       </c>
-      <c r="S2" s="135"/>
-      <c r="T2" s="136"/>
+      <c r="S2" s="134"/>
+      <c r="T2" s="135"/>
       <c r="U2" s="27" t="s">
         <v>62</v>
       </c>
@@ -22577,7 +22577,7 @@
       <c r="DG2" s="30"/>
     </row>
     <row r="3" spans="1:111" ht="21" customHeight="1">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="129" t="s">
         <v>66</v>
       </c>
       <c r="B3" s="31" t="s">
@@ -22592,21 +22592,21 @@
       <c r="G3" s="33"/>
       <c r="H3" s="33"/>
       <c r="I3" s="33"/>
-      <c r="J3" s="141" t="s">
+      <c r="J3" s="140" t="s">
         <v>68</v>
       </c>
-      <c r="K3" s="142"/>
-      <c r="L3" s="143"/>
-      <c r="M3" s="144"/>
-      <c r="N3" s="143"/>
-      <c r="O3" s="141" t="s">
+      <c r="K3" s="141"/>
+      <c r="L3" s="142"/>
+      <c r="M3" s="143"/>
+      <c r="N3" s="142"/>
+      <c r="O3" s="140" t="s">
         <v>68</v>
       </c>
-      <c r="P3" s="142"/>
-      <c r="Q3" s="143"/>
-      <c r="R3" s="141"/>
-      <c r="S3" s="142"/>
-      <c r="T3" s="142"/>
+      <c r="P3" s="141"/>
+      <c r="Q3" s="142"/>
+      <c r="R3" s="140"/>
+      <c r="S3" s="141"/>
+      <c r="T3" s="141"/>
       <c r="U3" s="34"/>
       <c r="V3" s="34"/>
       <c r="W3" s="34"/>
@@ -22700,7 +22700,7 @@
       <c r="DG3" s="15"/>
     </row>
     <row r="4" spans="1:111" ht="21" customHeight="1">
-      <c r="A4" s="131"/>
+      <c r="A4" s="130"/>
       <c r="B4" s="35" t="s">
         <v>69</v>
       </c>
@@ -22715,19 +22715,19 @@
       <c r="G4" s="37"/>
       <c r="H4" s="37"/>
       <c r="I4" s="37"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="111"/>
-      <c r="M4" s="125" t="s">
+      <c r="J4" s="144"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="N4" s="111"/>
-      <c r="O4" s="126"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="111"/>
-      <c r="R4" s="126"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="144"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="144"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
       <c r="U4" s="34"/>
       <c r="V4" s="34"/>
       <c r="W4" s="34"/>
@@ -22821,7 +22821,7 @@
       <c r="DG4" s="15"/>
     </row>
     <row r="5" spans="1:111" ht="21" customHeight="1">
-      <c r="A5" s="131"/>
+      <c r="A5" s="130"/>
       <c r="B5" s="35" t="s">
         <v>70</v>
       </c>
@@ -22834,19 +22834,19 @@
       <c r="G5" s="38"/>
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
-      <c r="J5" s="126"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="111"/>
-      <c r="M5" s="125" t="s">
+      <c r="J5" s="144"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="87"/>
+      <c r="M5" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="N5" s="111"/>
-      <c r="O5" s="126"/>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="111"/>
-      <c r="R5" s="126"/>
-      <c r="S5" s="112"/>
-      <c r="T5" s="112"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="144"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="87"/>
+      <c r="R5" s="144"/>
+      <c r="S5" s="88"/>
+      <c r="T5" s="88"/>
       <c r="U5" s="34"/>
       <c r="V5" s="34"/>
       <c r="W5" s="34"/>
@@ -22940,7 +22940,7 @@
       <c r="DG5" s="15"/>
     </row>
     <row r="6" spans="1:111" ht="21" customHeight="1">
-      <c r="A6" s="131"/>
+      <c r="A6" s="130"/>
       <c r="B6" s="35" t="s">
         <v>71</v>
       </c>
@@ -22953,19 +22953,19 @@
       <c r="G6" s="38"/>
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="112"/>
-      <c r="L6" s="111"/>
-      <c r="M6" s="125" t="s">
+      <c r="J6" s="144"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="N6" s="111"/>
-      <c r="O6" s="126"/>
-      <c r="P6" s="112"/>
-      <c r="Q6" s="111"/>
-      <c r="R6" s="126"/>
-      <c r="S6" s="112"/>
-      <c r="T6" s="112"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="144"/>
+      <c r="P6" s="88"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="144"/>
+      <c r="S6" s="88"/>
+      <c r="T6" s="88"/>
       <c r="U6" s="34"/>
       <c r="V6" s="34"/>
       <c r="W6" s="34"/>
@@ -23059,7 +23059,7 @@
       <c r="DG6" s="15"/>
     </row>
     <row r="7" spans="1:111" ht="21" customHeight="1">
-      <c r="A7" s="131"/>
+      <c r="A7" s="130"/>
       <c r="B7" s="35" t="s">
         <v>72</v>
       </c>
@@ -23072,19 +23072,19 @@
       </c>
       <c r="H7" s="38"/>
       <c r="I7" s="38"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="111"/>
-      <c r="M7" s="125" t="s">
+      <c r="J7" s="144"/>
+      <c r="K7" s="88"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="N7" s="111"/>
-      <c r="O7" s="126"/>
-      <c r="P7" s="112"/>
-      <c r="Q7" s="111"/>
-      <c r="R7" s="126"/>
-      <c r="S7" s="112"/>
-      <c r="T7" s="112"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="144"/>
+      <c r="P7" s="88"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="144"/>
+      <c r="S7" s="88"/>
+      <c r="T7" s="88"/>
       <c r="U7" s="34"/>
       <c r="V7" s="34"/>
       <c r="W7" s="34"/>
@@ -23178,7 +23178,7 @@
       <c r="DG7" s="15"/>
     </row>
     <row r="8" spans="1:111" ht="21" customHeight="1">
-      <c r="A8" s="131"/>
+      <c r="A8" s="130"/>
       <c r="B8" s="35" t="s">
         <v>73</v>
       </c>
@@ -23191,19 +23191,19 @@
         <v>68</v>
       </c>
       <c r="I8" s="38"/>
-      <c r="J8" s="126"/>
-      <c r="K8" s="112"/>
-      <c r="L8" s="111"/>
-      <c r="M8" s="125" t="s">
+      <c r="J8" s="144"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="N8" s="111"/>
-      <c r="O8" s="127"/>
-      <c r="P8" s="112"/>
-      <c r="Q8" s="111"/>
-      <c r="R8" s="127"/>
-      <c r="S8" s="112"/>
-      <c r="T8" s="112"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="145"/>
+      <c r="P8" s="88"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="145"/>
+      <c r="S8" s="88"/>
+      <c r="T8" s="88"/>
       <c r="U8" s="34"/>
       <c r="V8" s="34"/>
       <c r="W8" s="34"/>
@@ -23297,7 +23297,7 @@
       <c r="DG8" s="15"/>
     </row>
     <row r="9" spans="1:111" ht="21" customHeight="1">
-      <c r="A9" s="132"/>
+      <c r="A9" s="131"/>
       <c r="B9" s="35" t="s">
         <v>74</v>
       </c>
@@ -23310,19 +23310,19 @@
       <c r="I9" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="126"/>
-      <c r="K9" s="112"/>
-      <c r="L9" s="111"/>
-      <c r="M9" s="125"/>
-      <c r="N9" s="111"/>
-      <c r="O9" s="125"/>
-      <c r="P9" s="112"/>
-      <c r="Q9" s="111"/>
-      <c r="R9" s="125" t="s">
+      <c r="J9" s="144"/>
+      <c r="K9" s="88"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="117"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="117"/>
+      <c r="P9" s="88"/>
+      <c r="Q9" s="87"/>
+      <c r="R9" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="S9" s="112"/>
-      <c r="T9" s="112"/>
+      <c r="S9" s="88"/>
+      <c r="T9" s="88"/>
       <c r="U9" s="34"/>
       <c r="V9" s="34"/>
       <c r="W9" s="34"/>
@@ -57530,6 +57530,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R5:T5"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="C1:I1"/>
@@ -57546,27 +57567,6 @@
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="R4:T4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="J8:L8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>